<commit_message>
I just adjusted the column widths
and it's easier to push that than not imo
</commit_message>
<xml_diff>
--- a/okapi_annotation_scores.xlsx
+++ b/okapi_annotation_scores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasminebenmessaoud/Library/CloudStorage/OneDrive-ITU/Projects in Data Science/Github/Okapi/ProjectsinDataScience2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luke0\OneDrive\Documents\GitHub\ProjectsinDataScience2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704D2F45-9EF8-024B-8687-B248A0959B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9317CE-43CD-4CC9-B0BC-8D8828403E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{9C4BEEDA-5338-44B3-A977-4AE6DB12A241}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9C4BEEDA-5338-44B3-A977-4AE6DB12A241}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -964,22 +964,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8887C438-770E-4A0F-9D3E-5C85B6160971}">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G114" sqref="G114"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="8" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+    <col min="7" max="8" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>88</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>96</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>98</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>99</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>103</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>105</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>108</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>111</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>113</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>114</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>115</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>116</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>117</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>118</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>121</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>124</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>125</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>126</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>127</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>129</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>130</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>131</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>132</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>133</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>134</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>135</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>137</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>138</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>139</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>140</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>141</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>142</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>144</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>145</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>146</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>147</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>148</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>150</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>151</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>153</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>154</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>156</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>158</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>159</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>161</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>162</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>163</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>164</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>166</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>167</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>170</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>171</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>172</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>173</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>174</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>175</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>176</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>177</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>178</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>179</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>180</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>181</v>
       </c>
@@ -3608,6 +3608,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E66DD963F24B2248AA5B3BA27CE1D4AF" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b3e7f1cfb47299e140ad1cbf75b14e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cee8e6a1-b45e-4447-84bd-05603a71121e" xmlns:ns4="c9de5e97-094a-499d-9348-18672c3b4ad7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="006c05c0bd7bee21f2832a32e68f84b4" ns3:_="" ns4:_="">
     <xsd:import namespace="cee8e6a1-b45e-4447-84bd-05603a71121e"/>
@@ -3796,15 +3805,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3814,6 +3814,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B18BA688-A7FA-4BD0-82DE-67E17BD853E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59152EA4-B539-4EA9-94A7-5CE28412F58A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3832,14 +3840,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B18BA688-A7FA-4BD0-82DE-67E17BD853E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6F4CADD-D3B1-41F7-8882-F646E0E2B966}">
   <ds:schemaRefs>

</xml_diff>